<commit_message>
fix DocumentFile bug and send it
</commit_message>
<xml_diff>
--- a/Alarm_bot/Excel-Files/{"$type": "User", "id": "1314892980", "accessHash": "4705660583401878808"}.xlsx
+++ b/Alarm_bot/Excel-Files/{"$type": "User", "id": "1314892980", "accessHash": "4705660583401878808"}.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>1397:6:12</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>1397:6:15</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +430,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>